<commit_message>
LG and Rrr results summarized; gait metric added to SS-FP file
</commit_message>
<xml_diff>
--- a/synthesis/Excel file for S-S forest plots.xlsx
+++ b/synthesis/Excel file for S-S forest plots.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>FEMALE</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>800+</t>
+  </si>
+  <si>
+    <t>cm/s</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>gait metric</t>
   </si>
 </sst>
 </file>
@@ -467,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,7 +492,7 @@
     <col min="12" max="20" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -508,7 +520,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="11" t="s">
@@ -545,8 +557,11 @@
         <v>17</v>
       </c>
       <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>19</v>
@@ -596,7 +611,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -642,8 +657,11 @@
       <c r="R4">
         <v>2.3119999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -689,8 +707,11 @@
       <c r="R5">
         <v>0.29899999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -736,8 +757,11 @@
       <c r="R6">
         <v>0.66700000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -759,8 +783,11 @@
       <c r="T7">
         <v>6.6630000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -806,8 +833,11 @@
       <c r="R8">
         <v>0.31900000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -853,8 +883,11 @@
       <c r="R9">
         <v>0.32700000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -888,8 +921,11 @@
       <c r="T10">
         <v>0.11899999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -935,10 +971,16 @@
       <c r="R11">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
+      </c>
+      <c r="U12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
misc (ref, ssfp, alt tab)
</commit_message>
<xml_diff>
--- a/synthesis/Excel file for S-S forest plots.xlsx
+++ b/synthesis/Excel file for S-S forest plots.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>FEMALE</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>gait metric</t>
+  </si>
+  <si>
+    <t>?check</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>average of max??</t>
+  </si>
+  <si>
+    <t>averageof max from each hand?</t>
   </si>
 </sst>
 </file>
@@ -479,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:T11"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,7 +513,7 @@
     <col min="12" max="20" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -520,7 +541,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="11" t="s">
@@ -560,8 +581,11 @@
       <c r="U2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>19</v>
@@ -610,8 +634,11 @@
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -660,8 +687,11 @@
       <c r="U4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -710,8 +740,11 @@
       <c r="U5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -758,10 +791,13 @@
         <v>0.66700000000000004</v>
       </c>
       <c r="U6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="V6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -786,8 +822,11 @@
       <c r="U7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -836,8 +875,11 @@
       <c r="U8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -886,8 +928,11 @@
       <c r="U9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -924,8 +969,11 @@
       <c r="U10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -974,8 +1022,11 @@
       <c r="U11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>

</xml_diff>